<commit_message>
Changing seperator for excel output to semi-colon
</commit_message>
<xml_diff>
--- a/1314F8W_demonstration.xlsx
+++ b/1314F8W_demonstration.xlsx
@@ -16,120 +16,234 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="239">
   <si>
     <t>000000000</t>
   </si>
   <si>
+    <t>000000000;000000049</t>
+  </si>
+  <si>
     <t>000000001</t>
   </si>
   <si>
+    <t>000000001;000000049</t>
+  </si>
+  <si>
     <t>000000002</t>
   </si>
   <si>
+    <t>000000002;000000049</t>
+  </si>
+  <si>
     <t>000000003</t>
   </si>
   <si>
+    <t>000000003;000000049</t>
+  </si>
+  <si>
     <t>000000004</t>
   </si>
   <si>
+    <t>000000004;000000049</t>
+  </si>
+  <si>
     <t>000000005</t>
   </si>
   <si>
+    <t>000000005;000000049</t>
+  </si>
+  <si>
     <t>000000006</t>
   </si>
   <si>
+    <t>000000006;000000049</t>
+  </si>
+  <si>
     <t>000000007</t>
   </si>
   <si>
+    <t>000000007;000000049</t>
+  </si>
+  <si>
     <t>000000008</t>
   </si>
   <si>
+    <t>000000008;000000049</t>
+  </si>
+  <si>
     <t>000000009</t>
   </si>
   <si>
+    <t>000000009;000000049</t>
+  </si>
+  <si>
     <t>000000010</t>
   </si>
   <si>
+    <t>000000010;000000049</t>
+  </si>
+  <si>
     <t>000000011</t>
   </si>
   <si>
+    <t>000000011;000000049</t>
+  </si>
+  <si>
     <t>000000012</t>
   </si>
   <si>
+    <t>000000012;000000049</t>
+  </si>
+  <si>
     <t>000000013</t>
   </si>
   <si>
+    <t>000000013;000000049</t>
+  </si>
+  <si>
     <t>000000014</t>
   </si>
   <si>
+    <t>000000014;000000049</t>
+  </si>
+  <si>
     <t>000000015</t>
   </si>
   <si>
+    <t>000000015;000000049</t>
+  </si>
+  <si>
     <t>000000016</t>
   </si>
   <si>
+    <t>000000016;000000049</t>
+  </si>
+  <si>
     <t>000000017</t>
   </si>
   <si>
+    <t>000000017;000000049</t>
+  </si>
+  <si>
     <t>000000018</t>
   </si>
   <si>
+    <t>000000018;000000049</t>
+  </si>
+  <si>
     <t>000000019</t>
   </si>
   <si>
+    <t>000000019;000000049</t>
+  </si>
+  <si>
     <t>000000020</t>
   </si>
   <si>
+    <t>000000020;000000049</t>
+  </si>
+  <si>
     <t>000000021</t>
   </si>
   <si>
+    <t>000000021;000000049</t>
+  </si>
+  <si>
     <t>000000022</t>
   </si>
   <si>
+    <t>000000022;000000049</t>
+  </si>
+  <si>
     <t>000000023</t>
   </si>
   <si>
+    <t>000000023;000000049</t>
+  </si>
+  <si>
     <t>000000024</t>
   </si>
   <si>
+    <t>000000024;000000049</t>
+  </si>
+  <si>
     <t>000000025</t>
   </si>
   <si>
+    <t>000000025;000000049</t>
+  </si>
+  <si>
     <t>000000026</t>
   </si>
   <si>
+    <t>000000026;000000049</t>
+  </si>
+  <si>
     <t>000000027</t>
   </si>
   <si>
+    <t>000000027;000000049</t>
+  </si>
+  <si>
     <t>000000028</t>
   </si>
   <si>
+    <t>000000028;000000049</t>
+  </si>
+  <si>
     <t>000000029</t>
   </si>
   <si>
+    <t>000000029;000000049</t>
+  </si>
+  <si>
     <t>000000030</t>
   </si>
   <si>
+    <t>000000030;000000049</t>
+  </si>
+  <si>
     <t>000000031</t>
   </si>
   <si>
+    <t>000000031;000000049</t>
+  </si>
+  <si>
     <t>000000032</t>
   </si>
   <si>
+    <t>000000032;000000049</t>
+  </si>
+  <si>
     <t>000000033</t>
   </si>
   <si>
+    <t>000000033;000000049</t>
+  </si>
+  <si>
     <t>000000034</t>
   </si>
   <si>
+    <t>000000034;000000049</t>
+  </si>
+  <si>
     <t>000000035</t>
   </si>
   <si>
+    <t>000000035;000000049</t>
+  </si>
+  <si>
     <t>000000036</t>
   </si>
   <si>
+    <t>000000036;000000049</t>
+  </si>
+  <si>
     <t>000000037</t>
+  </si>
+  <si>
+    <t>000000037;000000049</t>
   </si>
   <si>
     <t>000000038</t>
@@ -975,9 +1089,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:AM60"/>
   <sheetViews>
@@ -987,169 +1101,169 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="39" max="39" customWidth="true" width="9.1"/>
-    <col min="38" max="38" customWidth="true" width="9.1"/>
-    <col min="37" max="37" customWidth="true" width="9.1"/>
-    <col min="36" max="36" customWidth="true" width="9.1"/>
-    <col min="35" max="35" customWidth="true" width="9.1"/>
-    <col min="34" max="34" customWidth="true" width="9.1"/>
-    <col min="33" max="33" customWidth="true" width="9.1"/>
-    <col min="32" max="32" customWidth="true" width="9.1"/>
-    <col min="31" max="31" customWidth="true" width="9.1"/>
-    <col min="30" max="30" customWidth="true" width="9.1"/>
-    <col min="29" max="29" customWidth="true" width="9.1"/>
-    <col min="28" max="28" customWidth="true" width="9.1"/>
-    <col min="27" max="27" customWidth="true" width="9.1"/>
-    <col min="13" max="13" customWidth="true" width="9.1"/>
-    <col min="12" max="12" customWidth="true" width="9.1"/>
-    <col min="15" max="15" customWidth="true" width="9.1"/>
-    <col min="14" max="14" customWidth="true" width="9.1"/>
-    <col min="9" max="9" customWidth="true" width="9.1"/>
-    <col min="8" max="8" customWidth="true" width="9.1"/>
-    <col min="11" max="11" customWidth="true" width="9.1"/>
-    <col min="10" max="10" customWidth="true" width="9.1"/>
-    <col min="5" max="5" customWidth="true" width="9.1"/>
-    <col min="4" max="4" customWidth="true" width="9.1"/>
-    <col min="7" max="7" customWidth="true" width="9.1"/>
-    <col min="6" max="6" customWidth="true" width="9.1"/>
-    <col min="1" max="1" customWidth="true" width="9.1"/>
-    <col min="3" max="3" customWidth="true" width="9.1"/>
-    <col min="2" max="2" customWidth="true" width="9.1"/>
-    <col min="25" max="25" customWidth="true" width="9.1"/>
-    <col min="24" max="24" customWidth="true" width="9.1"/>
-    <col min="26" max="26" customWidth="true" width="9.1"/>
-    <col min="21" max="21" customWidth="true" width="9.1"/>
-    <col min="20" max="20" customWidth="true" width="9.1"/>
-    <col min="23" max="23" customWidth="true" width="9.1"/>
-    <col min="22" max="22" customWidth="true" width="9.1"/>
-    <col min="17" max="17" customWidth="true" width="9.1"/>
-    <col min="16" max="16" customWidth="true" width="9.1"/>
-    <col min="19" max="19" customWidth="true" width="9.1"/>
-    <col min="18" max="18" customWidth="true" width="9.1"/>
+    <col min="12" width="9.1" customWidth="true" max="12"/>
+    <col min="13" width="9.1" customWidth="true" max="13"/>
+    <col min="14" width="9.1" customWidth="true" max="14"/>
+    <col min="15" width="9.1" customWidth="true" max="15"/>
+    <col min="8" width="9.1" customWidth="true" max="8"/>
+    <col min="9" width="9.1" customWidth="true" max="9"/>
+    <col min="10" width="9.1" customWidth="true" max="10"/>
+    <col min="11" width="9.1" customWidth="true" max="11"/>
+    <col min="4" width="9.1" customWidth="true" max="4"/>
+    <col min="5" width="9.1" customWidth="true" max="5"/>
+    <col min="6" width="9.1" customWidth="true" max="6"/>
+    <col min="7" width="9.1" customWidth="true" max="7"/>
+    <col min="1" width="9.1" customWidth="true" max="1"/>
+    <col min="2" width="9.1" customWidth="true" max="2"/>
+    <col min="3" width="9.1" customWidth="true" max="3"/>
+    <col min="36" width="9.1" customWidth="true" max="36"/>
+    <col min="28" width="9.1" customWidth="true" max="28"/>
+    <col min="34" width="9.1" customWidth="true" max="34"/>
+    <col min="35" width="9.1" customWidth="true" max="35"/>
+    <col min="24" width="9.1" customWidth="true" max="24"/>
+    <col min="25" width="9.1" customWidth="true" max="25"/>
+    <col min="26" width="9.1" customWidth="true" max="26"/>
+    <col min="29" width="9.1" customWidth="true" max="29"/>
+    <col min="20" width="9.1" customWidth="true" max="20"/>
+    <col min="21" width="9.1" customWidth="true" max="21"/>
+    <col min="22" width="9.1" customWidth="true" max="22"/>
+    <col min="23" width="9.1" customWidth="true" max="23"/>
+    <col min="16" width="9.1" customWidth="true" max="16"/>
+    <col min="17" width="9.1" customWidth="true" max="17"/>
+    <col min="18" width="9.1" customWidth="true" max="18"/>
+    <col min="19" width="9.1" customWidth="true" max="19"/>
+    <col min="27" width="9.1" customWidth="true" max="27"/>
+    <col min="39" width="9.1" customWidth="true" max="39"/>
+    <col min="37" width="9.1" customWidth="true" max="37"/>
+    <col min="32" width="9.1" customWidth="true" max="32"/>
+    <col min="33" width="9.1" customWidth="true" max="33"/>
+    <col min="30" width="9.1" customWidth="true" max="30"/>
+    <col min="38" width="9.1" customWidth="true" max="38"/>
+    <col min="31" width="9.1" customWidth="true" max="31"/>
   </cols>
   <sheetData>
-    <row spans="1:39" r="1">
-      <c s="1" t="s" r="A1">
-        <v>200</v>
-      </c>
-      <c s="1" t="n" r="B1">
-        <v>4.9e-08</v>
-      </c>
-      <c s="1" t="n" r="C1">
-        <v>1.000000049</v>
-      </c>
-      <c s="1" t="n" r="D1">
-        <v>2.000000049</v>
-      </c>
-      <c s="1" t="n" r="E1">
-        <v>3.000000049</v>
-      </c>
-      <c s="1" t="n" r="F1">
-        <v>4.000000049</v>
-      </c>
-      <c s="1" t="n" r="G1">
-        <v>5.000000049</v>
-      </c>
-      <c s="1" t="n" r="H1">
-        <v>6.000000049</v>
-      </c>
-      <c s="1" t="n" r="I1">
-        <v>7.000000049</v>
-      </c>
-      <c s="1" t="n" r="J1">
-        <v>8.000000049</v>
-      </c>
-      <c s="1" t="n" r="K1">
-        <v>9.000000049</v>
-      </c>
-      <c s="1" t="n" r="L1">
-        <v>10.000000049</v>
-      </c>
-      <c s="1" t="n" r="M1">
-        <v>11.000000049</v>
-      </c>
-      <c s="1" t="n" r="N1">
-        <v>12.000000049</v>
-      </c>
-      <c s="1" t="n" r="O1">
-        <v>13.000000049</v>
-      </c>
-      <c s="1" t="n" r="P1">
-        <v>14.000000049</v>
-      </c>
-      <c s="1" t="n" r="Q1">
-        <v>15.000000049</v>
-      </c>
-      <c s="1" t="n" r="R1">
-        <v>16.000000049</v>
-      </c>
-      <c s="1" t="n" r="S1">
-        <v>17.000000049</v>
-      </c>
-      <c s="1" t="n" r="T1">
-        <v>18.000000049</v>
-      </c>
-      <c s="1" t="n" r="U1">
-        <v>19.000000049</v>
-      </c>
-      <c s="1" t="n" r="V1">
-        <v>20.000000049</v>
-      </c>
-      <c s="1" t="n" r="W1">
-        <v>21.000000049</v>
-      </c>
-      <c s="1" t="n" r="X1">
-        <v>22.000000049</v>
-      </c>
-      <c s="1" t="n" r="Y1">
-        <v>23.000000049</v>
-      </c>
-      <c s="1" t="n" r="Z1">
-        <v>24.000000049</v>
-      </c>
-      <c s="1" t="n" r="AA1">
-        <v>25.000000049</v>
-      </c>
-      <c s="1" t="n" r="AB1">
-        <v>26.000000049</v>
-      </c>
-      <c s="1" t="n" r="AC1">
-        <v>27.000000049</v>
-      </c>
-      <c s="1" t="n" r="AD1">
-        <v>28.000000049</v>
-      </c>
-      <c s="1" t="n" r="AE1">
-        <v>29.000000049</v>
-      </c>
-      <c s="1" t="n" r="AF1">
-        <v>30.000000049</v>
-      </c>
-      <c s="1" t="n" r="AG1">
-        <v>31.000000049</v>
-      </c>
-      <c s="1" t="n" r="AH1">
-        <v>32.000000049</v>
-      </c>
-      <c s="1" t="n" r="AI1">
-        <v>33.000000049</v>
-      </c>
-      <c s="1" t="n" r="AJ1">
-        <v>34.000000049</v>
-      </c>
-      <c s="1" t="n" r="AK1">
-        <v>35.000000049</v>
-      </c>
-      <c s="1" t="n" r="AL1">
-        <v>36.000000049</v>
-      </c>
-      <c s="1" t="n" r="AM1">
-        <v>37.000000049</v>
-      </c>
-    </row>
-    <row spans="1:39" r="2">
-      <c s="1" t="s" r="A2">
-        <v>38</v>
+    <row r="1" spans="1:39">
+      <c t="s" r="A1" s="1">
+        <v>238</v>
+      </c>
+      <c t="s" r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c t="s" r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c t="s" r="D1" s="1">
+        <v>5</v>
+      </c>
+      <c t="s" r="E1" s="1">
+        <v>7</v>
+      </c>
+      <c t="s" r="F1" s="1">
+        <v>9</v>
+      </c>
+      <c t="s" r="G1" s="1">
+        <v>11</v>
+      </c>
+      <c t="s" r="H1" s="1">
+        <v>13</v>
+      </c>
+      <c t="s" r="I1" s="1">
+        <v>15</v>
+      </c>
+      <c t="s" r="J1" s="1">
+        <v>17</v>
+      </c>
+      <c t="s" r="K1" s="1">
+        <v>19</v>
+      </c>
+      <c t="s" r="L1" s="1">
+        <v>21</v>
+      </c>
+      <c t="s" r="M1" s="1">
+        <v>23</v>
+      </c>
+      <c t="s" r="N1" s="1">
+        <v>25</v>
+      </c>
+      <c t="s" r="O1" s="1">
+        <v>27</v>
+      </c>
+      <c t="s" r="P1" s="1">
+        <v>29</v>
+      </c>
+      <c t="s" r="Q1" s="1">
+        <v>31</v>
+      </c>
+      <c t="s" r="R1" s="1">
+        <v>33</v>
+      </c>
+      <c t="s" r="S1" s="1">
+        <v>35</v>
+      </c>
+      <c t="s" r="T1" s="1">
+        <v>37</v>
+      </c>
+      <c t="s" r="U1" s="1">
+        <v>39</v>
+      </c>
+      <c t="s" r="V1" s="1">
+        <v>41</v>
+      </c>
+      <c t="s" r="W1" s="1">
+        <v>43</v>
+      </c>
+      <c t="s" r="X1" s="1">
+        <v>45</v>
+      </c>
+      <c t="s" r="Y1" s="1">
+        <v>47</v>
+      </c>
+      <c t="s" r="Z1" s="1">
+        <v>49</v>
+      </c>
+      <c t="s" r="AA1" s="1">
+        <v>51</v>
+      </c>
+      <c t="s" r="AB1" s="1">
+        <v>53</v>
+      </c>
+      <c t="s" r="AC1" s="1">
+        <v>55</v>
+      </c>
+      <c t="s" r="AD1" s="1">
+        <v>57</v>
+      </c>
+      <c t="s" r="AE1" s="1">
+        <v>59</v>
+      </c>
+      <c t="s" r="AF1" s="1">
+        <v>61</v>
+      </c>
+      <c t="s" r="AG1" s="1">
+        <v>63</v>
+      </c>
+      <c t="s" r="AH1" s="1">
+        <v>65</v>
+      </c>
+      <c t="s" r="AI1" s="1">
+        <v>67</v>
+      </c>
+      <c t="s" r="AJ1" s="1">
+        <v>69</v>
+      </c>
+      <c t="s" r="AK1" s="1">
+        <v>71</v>
+      </c>
+      <c t="s" r="AL1" s="1">
+        <v>73</v>
+      </c>
+      <c t="s" r="AM1" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
+      <c t="s" r="A2" s="1">
+        <v>76</v>
       </c>
       <c t="n" r="B2">
         <v>0.15045871559633028</v>
@@ -1266,9 +1380,9 @@
         <v>0.3816280806572069</v>
       </c>
     </row>
-    <row spans="1:39" r="3">
-      <c s="1" t="s" r="A3">
-        <v>39</v>
+    <row r="3" spans="1:39">
+      <c t="s" r="A3" s="1">
+        <v>77</v>
       </c>
       <c t="n" r="B3">
         <v>0.3157894736842105</v>
@@ -1385,9 +1499,9 @@
         <v>0.38</v>
       </c>
     </row>
-    <row spans="1:39" r="4">
-      <c s="1" t="s" r="A4">
-        <v>40</v>
+    <row r="4" spans="1:39">
+      <c t="s" r="A4" s="1">
+        <v>78</v>
       </c>
       <c t="n" r="B4">
         <v>0.30333333333333334</v>
@@ -1504,9 +1618,9 @@
         <v>0.38109756097560976</v>
       </c>
     </row>
-    <row spans="1:39" r="5">
-      <c s="1" t="s" r="A5">
-        <v>41</v>
+    <row r="5" spans="1:39">
+      <c t="s" r="A5" s="1">
+        <v>79</v>
       </c>
       <c t="n" r="B5">
         <v>1.0</v>
@@ -1623,9 +1737,9 @@
         <v>0.6666666666666666</v>
       </c>
     </row>
-    <row spans="1:39" r="6">
-      <c s="1" t="s" r="A6">
-        <v>42</v>
+    <row r="6" spans="1:39">
+      <c t="s" r="A6" s="1">
+        <v>80</v>
       </c>
       <c t="n" r="B6">
         <v>0.3844221105527638</v>
@@ -1742,9 +1856,9 @@
         <v>0.3847715736040609</v>
       </c>
     </row>
-    <row spans="1:39" r="7">
-      <c s="1" t="s" r="A7">
-        <v>43</v>
+    <row r="7" spans="1:39">
+      <c t="s" r="A7" s="1">
+        <v>81</v>
       </c>
       <c t="n" r="B7">
         <v>0.30288461538461536</v>
@@ -1861,9 +1975,9 @@
         <v>0.3550863723608445</v>
       </c>
     </row>
-    <row spans="1:39" r="8">
-      <c s="1" t="s" r="A8">
-        <v>44</v>
+    <row r="8" spans="1:39">
+      <c t="s" r="A8" s="1">
+        <v>82</v>
       </c>
       <c t="n" r="B8">
         <v>0.3333333333333333</v>
@@ -1980,9 +2094,9 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row spans="1:39" r="9">
-      <c s="1" t="s" r="A9">
-        <v>45</v>
+    <row r="9" spans="1:39">
+      <c t="s" r="A9" s="1">
+        <v>83</v>
       </c>
       <c t="n" r="B9">
         <v>-1.0</v>
@@ -2090,9 +2204,9 @@
         <v>1.0</v>
       </c>
     </row>
-    <row spans="1:39" r="10">
-      <c s="1" t="s" r="A10">
-        <v>46</v>
+    <row r="10" spans="1:39">
+      <c t="s" r="A10" s="1">
+        <v>84</v>
       </c>
       <c t="n" r="B10">
         <v>0.34782608695652173</v>
@@ -2209,9 +2323,9 @@
         <v>0.3644859813084112</v>
       </c>
     </row>
-    <row spans="1:39" r="11">
-      <c s="1" t="s" r="A11">
-        <v>47</v>
+    <row r="11" spans="1:39">
+      <c t="s" r="A11" s="1">
+        <v>85</v>
       </c>
       <c t="n" r="B11">
         <v>0.0</v>
@@ -2328,9 +2442,9 @@
         <v>0.36774193548387096</v>
       </c>
     </row>
-    <row spans="1:39" r="12">
-      <c s="1" t="s" r="A12">
-        <v>48</v>
+    <row r="12" spans="1:39">
+      <c t="s" r="A12" s="1">
+        <v>86</v>
       </c>
       <c t="n" r="B12">
         <v>0.26186164433176384</v>
@@ -2447,9 +2561,9 @@
         <v>0.4023840206185567</v>
       </c>
     </row>
-    <row spans="1:39" r="13">
-      <c s="1" t="s" r="A13">
-        <v>50</v>
+    <row r="13" spans="1:39">
+      <c t="s" r="A13" s="1">
+        <v>88</v>
       </c>
       <c t="n" r="B13">
         <v>0.2903225806451613</v>
@@ -2563,9 +2677,9 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row spans="1:39" r="14">
-      <c s="1" t="s" r="A14">
-        <v>51</v>
+    <row r="14" spans="1:39">
+      <c t="s" r="A14" s="1">
+        <v>89</v>
       </c>
       <c t="n" r="B14">
         <v>0.23529411764705882</v>
@@ -2679,9 +2793,9 @@
         <v>0.23809523809523808</v>
       </c>
     </row>
-    <row spans="1:39" r="15">
-      <c s="1" t="s" r="A15">
-        <v>52</v>
+    <row r="15" spans="1:39">
+      <c t="s" r="A15" s="1">
+        <v>90</v>
       </c>
       <c t="n" r="B15">
         <v>0.29850746268656714</v>
@@ -2795,9 +2909,9 @@
         <v>0.2684563758389262</v>
       </c>
     </row>
-    <row spans="1:39" r="16">
-      <c s="1" t="s" r="A16">
-        <v>53</v>
+    <row r="16" spans="1:39">
+      <c t="s" r="A16" s="1">
+        <v>91</v>
       </c>
       <c t="n" r="B16">
         <v>0.4435483870967742</v>
@@ -2911,9 +3025,9 @@
         <v>0.5212765957446809</v>
       </c>
     </row>
-    <row spans="1:39" r="17">
-      <c s="1" t="s" r="A17">
-        <v>54</v>
+    <row r="17" spans="1:39">
+      <c t="s" r="A17" s="1">
+        <v>92</v>
       </c>
       <c t="n" r="B17">
         <v>0.38235294117647056</v>
@@ -3030,9 +3144,9 @@
         <v>0.2830188679245283</v>
       </c>
     </row>
-    <row spans="1:39" r="18">
-      <c s="1" t="s" r="A18">
-        <v>55</v>
+    <row r="18" spans="1:39">
+      <c t="s" r="A18" s="1">
+        <v>93</v>
       </c>
       <c t="n" r="B18">
         <v>0.026785714285714284</v>
@@ -3149,9 +3263,9 @@
         <v>0.5345622119815668</v>
       </c>
     </row>
-    <row spans="1:39" r="19">
-      <c s="1" t="s" r="A19">
-        <v>56</v>
+    <row r="19" spans="1:39">
+      <c t="s" r="A19" s="1">
+        <v>94</v>
       </c>
       <c t="n" r="B19">
         <v>0.2904761904761905</v>
@@ -3268,9 +3382,9 @@
         <v>0.4185185185185185</v>
       </c>
     </row>
-    <row spans="1:39" r="20">
-      <c s="1" t="s" r="A20">
-        <v>57</v>
+    <row r="20" spans="1:39">
+      <c t="s" r="A20" s="1">
+        <v>95</v>
       </c>
       <c t="n" r="B20">
         <v>0.2857142857142857</v>
@@ -3387,9 +3501,9 @@
         <v>0.2938775510204082</v>
       </c>
     </row>
-    <row spans="1:39" r="21">
-      <c s="1" t="s" r="A21">
-        <v>58</v>
+    <row r="21" spans="1:39">
+      <c t="s" r="A21" s="1">
+        <v>96</v>
       </c>
       <c t="n" r="B21">
         <v>0.36046511627906974</v>
@@ -3503,9 +3617,9 @@
         <v>0.38144329896907214</v>
       </c>
     </row>
-    <row spans="1:39" r="22">
-      <c s="1" t="s" r="A22">
-        <v>59</v>
+    <row r="22" spans="1:39">
+      <c t="s" r="A22" s="1">
+        <v>97</v>
       </c>
       <c t="n" r="B22">
         <v>0.3464566929133858</v>
@@ -3619,9 +3733,9 @@
         <v>0.33472803347280333</v>
       </c>
     </row>
-    <row spans="1:39" r="23">
-      <c s="1" t="s" r="A23">
-        <v>60</v>
+    <row r="23" spans="1:39">
+      <c t="s" r="A23" s="1">
+        <v>98</v>
       </c>
       <c t="n" r="B23">
         <v>0.07092198581560284</v>
@@ -3738,9 +3852,9 @@
         <v>0.6130536130536131</v>
       </c>
     </row>
-    <row spans="1:39" r="24">
-      <c s="1" t="s" r="A24">
-        <v>61</v>
+    <row r="24" spans="1:39">
+      <c t="s" r="A24" s="1">
+        <v>99</v>
       </c>
       <c t="n" r="B24">
         <v>-0.11538461538461539</v>
@@ -3854,9 +3968,9 @@
         <v>0.45</v>
       </c>
     </row>
-    <row spans="1:39" r="25">
-      <c s="1" t="s" r="A25">
-        <v>62</v>
+    <row r="25" spans="1:39">
+      <c t="s" r="A25" s="1">
+        <v>100</v>
       </c>
       <c t="n" r="B25">
         <v>0.19753086419753085</v>
@@ -3970,9 +4084,9 @@
         <v>0.43478260869565216</v>
       </c>
     </row>
-    <row spans="1:39" r="26">
-      <c s="1" t="s" r="A26">
-        <v>63</v>
+    <row r="26" spans="1:39">
+      <c t="s" r="A26" s="1">
+        <v>101</v>
       </c>
       <c t="n" r="B26">
         <v>0.3076923076923077</v>
@@ -4089,9 +4203,9 @@
         <v>0.34615384615384615</v>
       </c>
     </row>
-    <row spans="1:39" r="27">
-      <c s="1" t="s" r="A27">
-        <v>64</v>
+    <row r="27" spans="1:39">
+      <c t="s" r="A27" s="1">
+        <v>102</v>
       </c>
       <c t="n" r="B27">
         <v>0.2962962962962963</v>
@@ -4208,9 +4322,9 @@
         <v>0.467005076142132</v>
       </c>
     </row>
-    <row spans="1:39" r="28">
-      <c s="1" t="s" r="A28">
-        <v>65</v>
+    <row r="28" spans="1:39">
+      <c t="s" r="A28" s="1">
+        <v>103</v>
       </c>
       <c t="n" r="B28">
         <v>0.32727272727272727</v>
@@ -4324,9 +4438,9 @@
         <v>0.37333333333333335</v>
       </c>
     </row>
-    <row spans="1:39" r="29">
-      <c s="1" t="s" r="A29">
-        <v>66</v>
+    <row r="29" spans="1:39">
+      <c t="s" r="A29" s="1">
+        <v>104</v>
       </c>
       <c t="n" r="B29">
         <v>0.30097087378640774</v>
@@ -4440,9 +4554,9 @@
         <v>0.2328767123287671</v>
       </c>
     </row>
-    <row spans="1:39" r="30">
-      <c s="1" t="s" r="A30">
-        <v>67</v>
+    <row r="30" spans="1:39">
+      <c t="s" r="A30" s="1">
+        <v>105</v>
       </c>
       <c t="n" r="B30">
         <v>0.2692307692307692</v>
@@ -4556,9 +4670,9 @@
         <v>0.2692307692307692</v>
       </c>
     </row>
-    <row spans="1:39" r="31">
-      <c s="1" t="s" r="A31">
-        <v>68</v>
+    <row r="31" spans="1:39">
+      <c t="s" r="A31" s="1">
+        <v>106</v>
       </c>
       <c t="n" r="B31">
         <v>0.3155080213903743</v>
@@ -4675,9 +4789,9 @@
         <v>0.4650537634408602</v>
       </c>
     </row>
-    <row spans="1:39" r="32">
-      <c s="1" t="s" r="A32">
-        <v>69</v>
+    <row r="32" spans="1:39">
+      <c t="s" r="A32" s="1">
+        <v>107</v>
       </c>
       <c t="n" r="B32">
         <v>0.1875</v>
@@ -4791,9 +4905,9 @@
         <v>0.6494252873563219</v>
       </c>
     </row>
-    <row spans="1:39" r="33">
-      <c s="1" t="s" r="A33">
-        <v>70</v>
+    <row r="33" spans="1:39">
+      <c t="s" r="A33" s="1">
+        <v>108</v>
       </c>
       <c t="n" r="B33">
         <v>0.21348314606741572</v>
@@ -4907,9 +5021,9 @@
         <v>0.4712041884816754</v>
       </c>
     </row>
-    <row spans="1:39" r="34">
-      <c s="1" t="s" r="A34">
-        <v>71</v>
+    <row r="34" spans="1:39">
+      <c t="s" r="A34" s="1">
+        <v>109</v>
       </c>
       <c t="n" r="B34">
         <v>0.2153846153846154</v>
@@ -5023,9 +5137,9 @@
         <v>0.556390977443609</v>
       </c>
     </row>
-    <row spans="1:39" r="35">
-      <c s="1" t="s" r="A35">
-        <v>72</v>
+    <row r="35" spans="1:39">
+      <c t="s" r="A35" s="1">
+        <v>110</v>
       </c>
       <c t="n" r="B35">
         <v>0.27358490566037735</v>
@@ -5142,9 +5256,9 @@
         <v>0.3469387755102041</v>
       </c>
     </row>
-    <row spans="1:39" r="36">
-      <c s="1" t="s" r="A36">
-        <v>73</v>
+    <row r="36" spans="1:39">
+      <c t="s" r="A36" s="1">
+        <v>111</v>
       </c>
       <c t="n" r="B36">
         <v>0.3931034482758621</v>
@@ -5261,9 +5375,9 @@
         <v>0.4405144694533762</v>
       </c>
     </row>
-    <row spans="1:39" r="37">
-      <c s="1" t="s" r="A37">
-        <v>74</v>
+    <row r="37" spans="1:39">
+      <c t="s" r="A37" s="1">
+        <v>112</v>
       </c>
       <c t="n" r="B37">
         <v>0.5285714285714286</v>
@@ -5377,9 +5491,9 @@
         <v>0.5872093023255814</v>
       </c>
     </row>
-    <row spans="1:39" r="38">
-      <c s="1" t="s" r="A38">
-        <v>75</v>
+    <row r="38" spans="1:39">
+      <c t="s" r="A38" s="1">
+        <v>113</v>
       </c>
       <c t="n" r="B38">
         <v>0.008264462809917356</v>
@@ -5493,9 +5607,9 @@
         <v>0.3064516129032258</v>
       </c>
     </row>
-    <row spans="1:39" r="39">
-      <c s="1" t="s" r="A39">
-        <v>76</v>
+    <row r="39" spans="1:39">
+      <c t="s" r="A39" s="1">
+        <v>114</v>
       </c>
       <c t="n" r="B39">
         <v>0.203125</v>
@@ -5612,9 +5726,9 @@
         <v>0.16791044776119404</v>
       </c>
     </row>
-    <row spans="1:39" r="40">
-      <c s="1" t="s" r="A40">
-        <v>77</v>
+    <row r="40" spans="1:39">
+      <c t="s" r="A40" s="1">
+        <v>115</v>
       </c>
       <c t="n" r="B40">
         <v>0.11290322580645161</v>
@@ -5728,9 +5842,9 @@
         <v>0.10273972602739725</v>
       </c>
     </row>
-    <row spans="1:39" r="41">
-      <c s="1" t="s" r="A41">
-        <v>78</v>
+    <row r="41" spans="1:39">
+      <c t="s" r="A41" s="1">
+        <v>116</v>
       </c>
       <c t="n" r="B41">
         <v>0.14705882352941177</v>
@@ -5844,9 +5958,9 @@
         <v>0.5943396226415094</v>
       </c>
     </row>
-    <row spans="1:39" r="42">
-      <c s="1" t="s" r="A42">
-        <v>79</v>
+    <row r="42" spans="1:39">
+      <c t="s" r="A42" s="1">
+        <v>117</v>
       </c>
       <c t="n" r="B42">
         <v>-0.014492753623188406</v>
@@ -5960,9 +6074,9 @@
         <v>0.364741641337386</v>
       </c>
     </row>
-    <row spans="1:39" r="43">
-      <c s="1" t="s" r="A43">
-        <v>80</v>
+    <row r="43" spans="1:39">
+      <c t="s" r="A43" s="1">
+        <v>118</v>
       </c>
       <c t="n" r="B43">
         <v>0.52</v>
@@ -6076,9 +6190,9 @@
         <v>0.5454545454545454</v>
       </c>
     </row>
-    <row spans="1:39" r="44">
-      <c s="1" t="s" r="A44">
-        <v>81</v>
+    <row r="44" spans="1:39">
+      <c t="s" r="A44" s="1">
+        <v>119</v>
       </c>
       <c t="n" r="B44">
         <v>0.2711864406779661</v>
@@ -6192,9 +6306,9 @@
         <v>0.30612244897959184</v>
       </c>
     </row>
-    <row spans="1:39" r="45">
-      <c s="1" t="s" r="A45">
-        <v>82</v>
+    <row r="45" spans="1:39">
+      <c t="s" r="A45" s="1">
+        <v>120</v>
       </c>
       <c t="n" r="B45">
         <v>0.39920948616600793</v>
@@ -6311,9 +6425,9 @@
         <v>0.30095541401273884</v>
       </c>
     </row>
-    <row spans="1:39" r="46">
-      <c s="1" t="s" r="A46">
-        <v>83</v>
+    <row r="46" spans="1:39">
+      <c t="s" r="A46" s="1">
+        <v>121</v>
       </c>
       <c t="n" r="B46">
         <v>-0.12195121951219512</v>
@@ -6427,9 +6541,9 @@
         <v>0.4117647058823529</v>
       </c>
     </row>
-    <row spans="1:39" r="47">
-      <c s="1" t="s" r="A47">
-        <v>84</v>
+    <row r="47" spans="1:39">
+      <c t="s" r="A47" s="1">
+        <v>122</v>
       </c>
       <c t="n" r="B47">
         <v>0.08955223880597014</v>
@@ -6543,9 +6657,9 @@
         <v>0.27639751552795033</v>
       </c>
     </row>
-    <row spans="1:39" r="48">
-      <c s="1" t="s" r="A48">
-        <v>85</v>
+    <row r="48" spans="1:39">
+      <c t="s" r="A48" s="1">
+        <v>123</v>
       </c>
       <c t="n" r="B48">
         <v>0.2621359223300971</v>
@@ -6662,9 +6776,9 @@
         <v>0.4889867841409692</v>
       </c>
     </row>
-    <row spans="1:39" r="49">
-      <c s="1" t="s" r="A49">
-        <v>86</v>
+    <row r="49" spans="1:39">
+      <c t="s" r="A49" s="1">
+        <v>124</v>
       </c>
       <c t="n" r="B49">
         <v>0.6818181818181818</v>
@@ -6778,9 +6892,9 @@
         <v>0.37037037037037035</v>
       </c>
     </row>
-    <row spans="1:39" r="50">
-      <c s="1" t="s" r="A50">
-        <v>87</v>
+    <row r="50" spans="1:39">
+      <c t="s" r="A50" s="1">
+        <v>125</v>
       </c>
       <c t="n" r="B50">
         <v>0.2923076923076923</v>
@@ -6897,9 +7011,9 @@
         <v>0.5945945945945946</v>
       </c>
     </row>
-    <row spans="1:39" r="51">
-      <c s="1" t="s" r="A51">
-        <v>88</v>
+    <row r="51" spans="1:39">
+      <c t="s" r="A51" s="1">
+        <v>126</v>
       </c>
       <c t="n" r="B51">
         <v>0.6</v>
@@ -7016,9 +7130,9 @@
         <v>0.47368421052631576</v>
       </c>
     </row>
-    <row spans="1:39" r="52">
-      <c s="1" t="s" r="A52">
-        <v>89</v>
+    <row r="52" spans="1:39">
+      <c t="s" r="A52" s="1">
+        <v>127</v>
       </c>
       <c t="n" r="B52">
         <v>0.3069306930693069</v>
@@ -7135,9 +7249,9 @@
         <v>0.4528301886792453</v>
       </c>
     </row>
-    <row spans="1:39" r="53">
-      <c s="1" t="s" r="A53">
-        <v>90</v>
+    <row r="53" spans="1:39">
+      <c t="s" r="A53" s="1">
+        <v>128</v>
       </c>
       <c t="n" r="B53">
         <v>0.3225806451612903</v>
@@ -7254,9 +7368,9 @@
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row spans="1:39" r="54">
-      <c s="1" t="s" r="A54">
-        <v>91</v>
+    <row r="54" spans="1:39">
+      <c t="s" r="A54" s="1">
+        <v>129</v>
       </c>
       <c t="n" r="B54">
         <v>0.5416666666666666</v>
@@ -7370,9 +7484,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row spans="1:39" r="55">
-      <c s="1" t="s" r="A55">
-        <v>92</v>
+    <row r="55" spans="1:39">
+      <c t="s" r="A55" s="1">
+        <v>130</v>
       </c>
       <c t="n" r="B55">
         <v>0.12</v>
@@ -7489,9 +7603,9 @@
         <v>-0.058823529411764705</v>
       </c>
     </row>
-    <row spans="1:39" r="56">
-      <c s="1" t="s" r="A56">
-        <v>93</v>
+    <row r="56" spans="1:39">
+      <c t="s" r="A56" s="1">
+        <v>131</v>
       </c>
       <c t="n" r="B56">
         <v>0.1</v>
@@ -7605,9 +7719,9 @@
         <v>0.6486486486486487</v>
       </c>
     </row>
-    <row spans="1:39" r="57">
-      <c s="1" t="s" r="A57">
-        <v>94</v>
+    <row r="57" spans="1:39">
+      <c t="s" r="A57" s="1">
+        <v>132</v>
       </c>
       <c t="n" r="B57">
         <v>0.13846153846153847</v>
@@ -7721,9 +7835,9 @@
         <v>0.5586206896551724</v>
       </c>
     </row>
-    <row spans="1:39" r="58">
-      <c s="1" t="s" r="A58">
-        <v>95</v>
+    <row r="58" spans="1:39">
+      <c t="s" r="A58" s="1">
+        <v>133</v>
       </c>
       <c t="n" r="B58">
         <v>0.5517241379310345</v>
@@ -7837,9 +7951,9 @@
         <v>0.3880597014925373</v>
       </c>
     </row>
-    <row spans="1:39" r="59">
-      <c s="1" t="s" r="A59">
-        <v>96</v>
+    <row r="59" spans="1:39">
+      <c t="s" r="A59" s="1">
+        <v>134</v>
       </c>
       <c t="n" r="B59">
         <v>0.5</v>
@@ -7953,9 +8067,9 @@
         <v>0.6052631578947368</v>
       </c>
     </row>
-    <row spans="1:39" r="60">
-      <c s="1" t="s" r="A60">
-        <v>97</v>
+    <row r="60" spans="1:39">
+      <c t="s" r="A60" s="1">
+        <v>135</v>
       </c>
       <c t="n" r="E60">
         <v>0.7777777777777778</v>
@@ -8053,9 +8167,9 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
@@ -8065,1102 +8179,1102 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="4" max="4" width="9.10"/>
     <col min="5" max="5" width="9.10"/>
-    <col min="4" max="4" width="9.10"/>
     <col min="6" max="6" width="9.10"/>
     <col min="1" max="1" width="9.10"/>
+    <col min="2" max="2" width="9.10"/>
     <col min="3" max="3" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
   </cols>
   <sheetData>
-    <row spans="1:6" r="1">
+    <row r="1" spans="1:6">
       <c t="s" r="A1">
-        <v>147</v>
+        <v>234</v>
       </c>
       <c t="s" r="B1">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c t="s" r="C1">
-        <v>198</v>
+        <v>237</v>
       </c>
       <c t="s" r="D1">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c t="s" r="E1">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c t="s" r="F1">
-        <v>195</v>
-      </c>
-    </row>
-    <row spans="1:6" r="2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c t="s" r="A2">
-        <v>144</v>
+        <v>201</v>
       </c>
       <c t="s" r="B2">
+        <v>120</v>
+      </c>
+      <c t="s" r="C2">
+        <v>87</v>
+      </c>
+      <c t="s" r="D2">
+        <v>120</v>
+      </c>
+      <c t="s" r="E2">
+        <v>76</v>
+      </c>
+      <c t="s" r="F2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c t="s" r="A3">
+        <v>224</v>
+      </c>
+      <c t="s" r="B3">
+        <v>130</v>
+      </c>
+      <c t="s" r="D3">
+        <v>130</v>
+      </c>
+      <c t="s" r="E3">
+        <v>78</v>
+      </c>
+      <c t="s" r="F3">
         <v>66</v>
       </c>
-      <c t="s" r="C2">
-        <v>69</v>
-      </c>
-      <c t="s" r="D2">
-        <v>49</v>
-      </c>
-      <c t="s" r="E2">
-        <v>13</v>
-      </c>
-      <c t="s" r="F2">
-        <v>39</v>
-      </c>
-    </row>
-    <row spans="1:6" r="3">
-      <c t="s" r="A3">
-        <v>161</v>
-      </c>
-      <c t="s" r="B3">
+    </row>
+    <row r="4" spans="1:6">
+      <c t="s" r="A4">
+        <v>219</v>
+      </c>
+      <c t="s" r="B4">
+        <v>126</v>
+      </c>
+      <c t="s" r="D4">
+        <v>126</v>
+      </c>
+      <c t="s" r="E4">
+        <v>79</v>
+      </c>
+      <c t="s" r="F4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c t="s" r="A5">
+        <v>167</v>
+      </c>
+      <c t="s" r="B5">
+        <v>93</v>
+      </c>
+      <c t="s" r="D5">
+        <v>93</v>
+      </c>
+      <c t="s" r="E5">
+        <v>85</v>
+      </c>
+      <c t="s" r="F5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c t="s" r="A6">
+        <v>185</v>
+      </c>
+      <c t="s" r="B6">
+        <v>107</v>
+      </c>
+      <c t="s" r="D6">
+        <v>107</v>
+      </c>
+      <c t="s" r="E6">
         <v>80</v>
       </c>
-      <c t="s" r="C3">
-        <v>66</v>
-      </c>
-      <c t="s" r="E3">
-        <v>14</v>
-      </c>
-      <c t="s" r="F3">
-        <v>45</v>
-      </c>
-    </row>
-    <row spans="1:6" r="4">
-      <c t="s" r="A4">
-        <v>190</v>
-      </c>
-      <c t="s" r="B4">
-        <v>96</v>
-      </c>
-      <c t="s" r="C4">
-        <v>80</v>
-      </c>
-      <c t="s" r="E4">
-        <v>4</v>
-      </c>
-      <c t="s" r="F4">
-        <v>41</v>
-      </c>
-    </row>
-    <row spans="1:6" r="5">
-      <c t="s" r="A5">
-        <v>162</v>
-      </c>
-      <c t="s" r="B5">
+      <c t="s" r="F6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c t="s" r="A7">
+        <v>228</v>
+      </c>
+      <c t="s" r="B7">
+        <v>134</v>
+      </c>
+      <c t="s" r="D7">
+        <v>134</v>
+      </c>
+      <c t="s" r="E7">
         <v>81</v>
       </c>
-      <c t="s" r="C5">
-        <v>96</v>
-      </c>
-      <c t="s" r="E5">
-        <v>36</v>
-      </c>
-      <c t="s" r="F5">
-        <v>40</v>
-      </c>
-    </row>
-    <row spans="1:6" r="6">
-      <c t="s" r="A6">
-        <v>132</v>
-      </c>
-      <c t="s" r="B6">
-        <v>58</v>
-      </c>
-      <c t="s" r="C6">
-        <v>81</v>
-      </c>
-      <c t="s" r="E6">
-        <v>7</v>
-      </c>
-      <c t="s" r="F6">
-        <v>44</v>
-      </c>
-    </row>
-    <row spans="1:6" r="7">
-      <c t="s" r="A7">
-        <v>149</v>
-      </c>
-      <c t="s" r="B7">
-        <v>71</v>
-      </c>
-      <c t="s" r="C7">
-        <v>58</v>
-      </c>
-      <c t="s" r="E7">
-        <v>12</v>
-      </c>
       <c t="s" r="F7">
-        <v>43</v>
-      </c>
-    </row>
-    <row spans="1:6" r="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c t="s" r="A8">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c t="s" r="B8">
         <v>97</v>
       </c>
-      <c t="s" r="C8">
-        <v>71</v>
+      <c t="s" r="D8">
+        <v>97</v>
       </c>
       <c t="s" r="E8">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c t="s" r="F8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c t="s" r="A9">
+        <v>200</v>
+      </c>
+      <c t="s" r="B9">
+        <v>119</v>
+      </c>
+      <c t="s" r="D9">
+        <v>119</v>
+      </c>
+      <c t="s" r="E9">
+        <v>86</v>
+      </c>
+      <c t="s" r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c t="s" r="A10">
+        <v>174</v>
+      </c>
+      <c t="s" r="B10">
+        <v>99</v>
+      </c>
+      <c t="s" r="D10">
+        <v>99</v>
+      </c>
+      <c t="s" r="E10">
+        <v>77</v>
+      </c>
+      <c t="s" r="F10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c t="s" r="A11">
+        <v>225</v>
+      </c>
+      <c t="s" r="B11">
+        <v>131</v>
+      </c>
+      <c t="s" r="D11">
+        <v>131</v>
+      </c>
+      <c t="s" r="E11">
+        <v>83</v>
+      </c>
+      <c t="s" r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c t="s" r="A12">
+        <v>209</v>
+      </c>
+      <c t="s" r="B12">
+        <v>123</v>
+      </c>
+      <c t="s" r="D12">
+        <v>123</v>
+      </c>
+      <c t="s" r="E12">
+        <v>84</v>
+      </c>
+      <c t="s" r="F12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c t="s" r="A13">
+        <v>217</v>
+      </c>
+      <c t="s" r="B13">
+        <v>124</v>
+      </c>
+      <c t="s" r="D13">
+        <v>124</v>
+      </c>
+      <c t="s" r="F13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c t="s" r="A14">
+        <v>181</v>
+      </c>
+      <c t="s" r="B14">
+        <v>103</v>
+      </c>
+      <c t="s" r="D14">
+        <v>103</v>
+      </c>
+      <c t="s" r="F14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c t="s" r="A15">
+        <v>190</v>
+      </c>
+      <c t="s" r="B15">
+        <v>111</v>
+      </c>
+      <c t="s" r="D15">
+        <v>111</v>
+      </c>
+      <c t="s" r="F15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c t="s" r="A16">
+        <v>202</v>
+      </c>
+      <c t="s" r="B16">
+        <v>121</v>
+      </c>
+      <c t="s" r="D16">
+        <v>121</v>
+      </c>
+      <c t="s" r="F16">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c t="s" r="A17">
+        <v>180</v>
+      </c>
+      <c t="s" r="B17">
+        <v>102</v>
+      </c>
+      <c t="s" r="D17">
+        <v>102</v>
+      </c>
+      <c t="s" r="F17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c t="s" r="A18">
+        <v>182</v>
+      </c>
+      <c t="s" r="B18">
+        <v>104</v>
+      </c>
+      <c t="s" r="D18">
+        <v>104</v>
+      </c>
+      <c t="s" r="F18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c t="s" r="A19">
+        <v>143</v>
+      </c>
+      <c t="s" r="B19">
+        <v>90</v>
+      </c>
+      <c t="s" r="D19">
+        <v>90</v>
+      </c>
+      <c t="s" r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c t="s" r="A20">
+        <v>195</v>
+      </c>
+      <c t="s" r="B20">
+        <v>116</v>
+      </c>
+      <c t="s" r="D20">
+        <v>116</v>
+      </c>
+      <c t="s" r="F20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c t="s" r="A21">
+        <v>183</v>
+      </c>
+      <c t="s" r="B21">
+        <v>105</v>
+      </c>
+      <c t="s" r="D21">
+        <v>105</v>
+      </c>
+      <c t="s" r="F21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c t="s" r="A22">
+        <v>222</v>
+      </c>
+      <c t="s" r="B22">
+        <v>128</v>
+      </c>
+      <c t="s" r="D22">
+        <v>128</v>
+      </c>
+      <c t="s" r="F22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c t="s" r="A23">
+        <v>187</v>
+      </c>
+      <c t="s" r="B23">
+        <v>109</v>
+      </c>
+      <c t="s" r="D23">
+        <v>109</v>
+      </c>
+      <c t="s" r="F23">
         <v>48</v>
       </c>
     </row>
-    <row spans="1:6" r="9">
-      <c t="s" r="A9">
+    <row r="24" spans="1:6">
+      <c t="s" r="A24">
+        <v>186</v>
+      </c>
+      <c t="s" r="B24">
+        <v>108</v>
+      </c>
+      <c t="s" r="D24">
+        <v>108</v>
+      </c>
+      <c t="s" r="F24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c t="s" r="A25">
+        <v>142</v>
+      </c>
+      <c t="s" r="B25">
+        <v>89</v>
+      </c>
+      <c t="s" r="D25">
+        <v>89</v>
+      </c>
+      <c t="s" r="F25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c t="s" r="A26">
+        <v>175</v>
+      </c>
+      <c t="s" r="B26">
+        <v>100</v>
+      </c>
+      <c t="s" r="D26">
+        <v>100</v>
+      </c>
+      <c t="s" r="F26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c t="s" r="A27">
+        <v>168</v>
+      </c>
+      <c t="s" r="B27">
+        <v>94</v>
+      </c>
+      <c t="s" r="D27">
+        <v>94</v>
+      </c>
+      <c t="s" r="F27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c t="s" r="A28">
+        <v>220</v>
+      </c>
+      <c t="s" r="B28">
+        <v>127</v>
+      </c>
+      <c t="s" r="D28">
+        <v>127</v>
+      </c>
+      <c t="s" r="F28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c t="s" r="A29">
+        <v>221</v>
+      </c>
+      <c t="s" r="B29">
+        <v>135</v>
+      </c>
+      <c t="s" r="D29">
+        <v>135</v>
+      </c>
+      <c t="s" r="F29">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c t="s" r="A30">
+        <v>170</v>
+      </c>
+      <c t="s" r="B30">
+        <v>96</v>
+      </c>
+      <c t="s" r="D30">
+        <v>96</v>
+      </c>
+      <c t="s" r="F30">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c t="s" r="A31">
+        <v>169</v>
+      </c>
+      <c t="s" r="B31">
+        <v>95</v>
+      </c>
+      <c t="s" r="D31">
+        <v>95</v>
+      </c>
+      <c t="s" r="F31">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c t="s" r="A32">
+        <v>194</v>
+      </c>
+      <c t="s" r="B32">
+        <v>115</v>
+      </c>
+      <c t="s" r="D32">
+        <v>115</v>
+      </c>
+      <c t="s" r="F32">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c t="s" r="A33">
+        <v>193</v>
+      </c>
+      <c t="s" r="B33">
+        <v>114</v>
+      </c>
+      <c t="s" r="D33">
+        <v>114</v>
+      </c>
+      <c t="s" r="F33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c t="s" r="A34">
+        <v>137</v>
+      </c>
+      <c t="s" r="B34">
+        <v>88</v>
+      </c>
+      <c t="s" r="D34">
+        <v>88</v>
+      </c>
+      <c t="s" r="F34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c t="s" r="A35">
+        <v>218</v>
+      </c>
+      <c t="s" r="B35">
+        <v>125</v>
+      </c>
+      <c t="s" r="D35">
+        <v>125</v>
+      </c>
+      <c t="s" r="F35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c t="s" r="A36">
+        <v>192</v>
+      </c>
+      <c t="s" r="B36">
+        <v>113</v>
+      </c>
+      <c t="s" r="D36">
+        <v>113</v>
+      </c>
+      <c t="s" r="F36">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c t="s" r="A37">
+        <v>184</v>
+      </c>
+      <c t="s" r="B37">
+        <v>106</v>
+      </c>
+      <c t="s" r="D37">
+        <v>106</v>
+      </c>
+      <c t="s" r="F37">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c t="s" r="A38">
+        <v>227</v>
+      </c>
+      <c t="s" r="B38">
+        <v>133</v>
+      </c>
+      <c t="s" r="D38">
+        <v>133</v>
+      </c>
+      <c t="s" r="F38">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c t="s" r="A39">
+        <v>176</v>
+      </c>
+      <c t="s" r="B39">
+        <v>101</v>
+      </c>
+      <c t="s" r="D39">
+        <v>101</v>
+      </c>
+      <c t="s" r="F39">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c t="s" r="A40">
+        <v>203</v>
+      </c>
+      <c t="s" r="B40">
+        <v>122</v>
+      </c>
+      <c t="s" r="D40">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c t="s" r="A41">
+        <v>223</v>
+      </c>
+      <c t="s" r="B41">
+        <v>129</v>
+      </c>
+      <c t="s" r="D41">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c t="s" r="A42">
+        <v>146</v>
+      </c>
+      <c t="s" r="B42">
+        <v>91</v>
+      </c>
+      <c t="s" r="D42">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c t="s" r="A43">
+        <v>188</v>
+      </c>
+      <c t="s" r="B43">
+        <v>110</v>
+      </c>
+      <c t="s" r="D43">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c t="s" r="A44">
+        <v>173</v>
+      </c>
+      <c t="s" r="B44">
+        <v>98</v>
+      </c>
+      <c t="s" r="D44">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c t="s" r="A45">
+        <v>147</v>
+      </c>
+      <c t="s" r="B45">
+        <v>92</v>
+      </c>
+      <c t="s" r="D45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c t="s" r="A46">
+        <v>226</v>
+      </c>
+      <c t="s" r="B46">
+        <v>132</v>
+      </c>
+      <c t="s" r="D46">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c t="s" r="A47">
+        <v>196</v>
+      </c>
+      <c t="s" r="B47">
+        <v>117</v>
+      </c>
+      <c t="s" r="D47">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c t="s" r="A48">
+        <v>191</v>
+      </c>
+      <c t="s" r="B48">
+        <v>112</v>
+      </c>
+      <c t="s" r="D48">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c t="s" r="A49">
+        <v>199</v>
+      </c>
+      <c t="s" r="B49">
+        <v>118</v>
+      </c>
+      <c t="s" r="D49">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c t="s" r="A50">
+        <v>136</v>
+      </c>
+      <c t="s" r="B50">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c t="s" r="A51">
+        <v>144</v>
+      </c>
+      <c t="s" r="B51">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c t="s" r="A52">
         <v>145</v>
       </c>
-      <c t="s" r="B9">
-        <v>67</v>
-      </c>
-      <c t="s" r="C9">
-        <v>97</v>
-      </c>
-      <c t="s" r="E9">
-        <v>16</v>
-      </c>
-      <c t="s" r="F9">
-        <v>46</v>
-      </c>
-    </row>
-    <row spans="1:6" r="10">
-      <c t="s" r="A10">
-        <v>188</v>
-      </c>
-      <c t="s" r="B10">
-        <v>94</v>
-      </c>
-      <c t="s" r="C10">
-        <v>67</v>
-      </c>
-      <c t="s" r="E10">
-        <v>27</v>
-      </c>
-      <c t="s" r="F10">
-        <v>42</v>
-      </c>
-    </row>
-    <row spans="1:6" r="11">
-      <c t="s" r="A11">
+      <c t="s" r="B52">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c t="s" r="A53">
+        <v>206</v>
+      </c>
+      <c t="s" r="B53">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c t="s" r="A54">
         <v>189</v>
       </c>
-      <c t="s" r="B11">
-        <v>95</v>
-      </c>
-      <c t="s" r="C11">
-        <v>94</v>
-      </c>
-      <c t="s" r="E11">
-        <v>35</v>
-      </c>
-      <c t="s" r="F11">
-        <v>38</v>
-      </c>
-    </row>
-    <row spans="1:6" r="12">
-      <c t="s" r="A12">
-        <v>130</v>
-      </c>
-      <c t="s" r="B12">
-        <v>56</v>
-      </c>
-      <c t="s" r="C12">
-        <v>95</v>
-      </c>
-      <c t="s" r="E12">
-        <v>25</v>
-      </c>
-      <c t="s" r="F12">
-        <v>47</v>
-      </c>
-    </row>
-    <row spans="1:6" r="13">
-      <c t="s" r="A13">
-        <v>155</v>
-      </c>
-      <c t="s" r="B13">
-        <v>76</v>
-      </c>
-      <c t="s" r="C13">
-        <v>56</v>
-      </c>
-      <c t="s" r="E13">
-        <v>22</v>
-      </c>
-    </row>
-    <row spans="1:6" r="14">
-      <c t="s" r="A14">
-        <v>182</v>
-      </c>
-      <c t="s" r="B14">
-        <v>89</v>
-      </c>
-      <c t="s" r="C14">
-        <v>76</v>
-      </c>
-      <c t="s" r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row spans="1:6" r="15">
-      <c t="s" r="A15">
-        <v>108</v>
-      </c>
-      <c t="s" r="B15">
-        <v>53</v>
-      </c>
-      <c t="s" r="C15">
-        <v>89</v>
-      </c>
-      <c t="s" r="E15">
-        <v>31</v>
-      </c>
-    </row>
-    <row spans="1:6" r="16">
-      <c t="s" r="A16">
-        <v>129</v>
-      </c>
-      <c t="s" r="B16">
-        <v>55</v>
-      </c>
-      <c t="s" r="C16">
-        <v>53</v>
-      </c>
-      <c t="s" r="E16">
-        <v>32</v>
-      </c>
-    </row>
-    <row spans="1:6" r="17">
-      <c t="s" r="A17">
-        <v>185</v>
-      </c>
-      <c t="s" r="B17">
-        <v>91</v>
-      </c>
-      <c t="s" r="C17">
-        <v>55</v>
-      </c>
-      <c t="s" r="E17">
-        <v>33</v>
-      </c>
-    </row>
-    <row spans="1:6" r="18">
-      <c t="s" r="A18">
-        <v>138</v>
-      </c>
-      <c t="s" r="B18">
-        <v>63</v>
-      </c>
-      <c t="s" r="C18">
-        <v>91</v>
-      </c>
-      <c t="s" r="E18">
-        <v>34</v>
-      </c>
-    </row>
-    <row spans="1:6" r="19">
-      <c t="s" r="A19">
-        <v>109</v>
-      </c>
-      <c t="s" r="B19">
-        <v>54</v>
-      </c>
-      <c t="s" r="C19">
-        <v>63</v>
-      </c>
-      <c t="s" r="E19">
-        <v>28</v>
-      </c>
-    </row>
-    <row spans="1:6" r="20">
-      <c t="s" r="A20">
-        <v>131</v>
-      </c>
-      <c t="s" r="B20">
-        <v>57</v>
-      </c>
-      <c t="s" r="C20">
-        <v>54</v>
-      </c>
-      <c t="s" r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:6" r="21">
-      <c t="s" r="A21">
-        <v>186</v>
-      </c>
-      <c t="s" r="B21">
-        <v>92</v>
-      </c>
-      <c t="s" r="C21">
-        <v>57</v>
-      </c>
-      <c t="s" r="E21">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:6" r="22">
-      <c t="s" r="A22">
-        <v>105</v>
-      </c>
-      <c t="s" r="B22">
-        <v>52</v>
-      </c>
-      <c t="s" r="C22">
-        <v>92</v>
-      </c>
-      <c t="s" r="E22">
-        <v>24</v>
-      </c>
-    </row>
-    <row spans="1:6" r="23">
-      <c t="s" r="A23">
-        <v>181</v>
-      </c>
-      <c t="s" r="B23">
-        <v>88</v>
-      </c>
-      <c t="s" r="C23">
-        <v>52</v>
-      </c>
-      <c t="s" r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row spans="1:6" r="24">
-      <c t="s" r="A24">
-        <v>104</v>
-      </c>
-      <c t="s" r="B24">
-        <v>51</v>
-      </c>
-      <c t="s" r="C24">
-        <v>88</v>
-      </c>
-      <c t="s" r="E24">
-        <v>18</v>
-      </c>
-    </row>
-    <row spans="1:6" r="25">
-      <c t="s" r="A25">
-        <v>179</v>
-      </c>
-      <c t="s" r="B25">
+      <c t="s" r="B54">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c t="s" r="A55">
+        <v>197</v>
+      </c>
+      <c t="s" r="B55">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c t="s" r="A56">
+        <v>198</v>
+      </c>
+      <c t="s" r="B56">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c t="s" r="A57">
+        <v>229</v>
+      </c>
+      <c t="s" r="B57">
         <v>86</v>
       </c>
-      <c t="s" r="C25">
-        <v>51</v>
-      </c>
-      <c t="s" r="E25">
-        <v>10</v>
-      </c>
-    </row>
-    <row spans="1:6" r="26">
-      <c t="s" r="A26">
-        <v>171</v>
-      </c>
-      <c t="s" r="B26">
-        <v>85</v>
-      </c>
-      <c t="s" r="C26">
-        <v>86</v>
-      </c>
-      <c t="s" r="E26">
-        <v>15</v>
-      </c>
-    </row>
-    <row spans="1:6" r="27">
-      <c t="s" r="A27">
+    </row>
+    <row r="58" spans="1:6">
+      <c t="s" r="A58">
+        <v>141</v>
+      </c>
+      <c t="s" r="B58">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c t="s" r="A59">
+        <v>204</v>
+      </c>
+      <c t="s" r="B59">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c t="s" r="A60">
+        <v>205</v>
+      </c>
+      <c t="s" r="B60">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c t="s" r="A61">
+        <v>213</v>
+      </c>
+      <c t="s" r="B61">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c t="s" r="A62">
+        <v>215</v>
+      </c>
+      <c t="s" r="B62">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c t="s" r="A63">
+        <v>214</v>
+      </c>
+      <c t="s" r="B63">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c t="s" r="A64">
+        <v>216</v>
+      </c>
+      <c t="s" r="B64">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c t="s" r="A65">
+        <v>158</v>
+      </c>
+      <c t="s" r="B65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c t="s" r="A66">
         <v>148</v>
       </c>
-      <c t="s" r="B27">
-        <v>70</v>
-      </c>
-      <c t="s" r="C27">
-        <v>85</v>
-      </c>
-      <c t="s" r="E27">
-        <v>19</v>
-      </c>
-    </row>
-    <row spans="1:6" r="28">
-      <c t="s" r="A28">
-        <v>150</v>
-      </c>
-      <c t="s" r="B28">
-        <v>72</v>
-      </c>
-      <c t="s" r="C28">
-        <v>70</v>
-      </c>
-      <c t="s" r="E28">
-        <v>21</v>
-      </c>
-    </row>
-    <row spans="1:6" r="29">
-      <c t="s" r="A29">
-        <v>137</v>
-      </c>
-      <c t="s" r="B29">
-        <v>62</v>
-      </c>
-      <c t="s" r="C29">
-        <v>72</v>
-      </c>
-      <c t="s" r="E29">
-        <v>11</v>
-      </c>
-    </row>
-    <row spans="1:6" r="30">
-      <c t="s" r="A30">
-        <v>134</v>
-      </c>
-      <c t="s" r="B30">
-        <v>59</v>
-      </c>
-      <c t="s" r="C30">
-        <v>62</v>
-      </c>
-      <c t="s" r="E30">
-        <v>23</v>
-      </c>
-    </row>
-    <row spans="1:6" r="31">
-      <c t="s" r="A31">
-        <v>157</v>
-      </c>
-      <c t="s" r="B31">
-        <v>78</v>
-      </c>
-      <c t="s" r="C31">
-        <v>59</v>
-      </c>
-      <c t="s" r="E31">
-        <v>26</v>
-      </c>
-    </row>
-    <row spans="1:6" r="32">
-      <c t="s" r="A32">
-        <v>180</v>
-      </c>
-      <c t="s" r="B32">
-        <v>87</v>
-      </c>
-      <c t="s" r="C32">
-        <v>78</v>
-      </c>
-      <c t="s" r="E32">
-        <v>30</v>
-      </c>
-    </row>
-    <row spans="1:6" r="33">
-      <c t="s" r="A33">
-        <v>152</v>
-      </c>
-      <c t="s" r="B33">
-        <v>73</v>
-      </c>
-      <c t="s" r="C33">
-        <v>87</v>
-      </c>
-      <c t="s" r="E33">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:6" r="34">
-      <c t="s" r="A34">
-        <v>187</v>
-      </c>
-      <c t="s" r="B34">
-        <v>93</v>
-      </c>
-      <c t="s" r="C34">
-        <v>73</v>
-      </c>
-      <c t="s" r="E34">
-        <v>9</v>
-      </c>
-    </row>
-    <row spans="1:6" r="35">
-      <c t="s" r="A35">
-        <v>99</v>
-      </c>
-      <c t="s" r="B35">
-        <v>50</v>
-      </c>
-      <c t="s" r="C35">
-        <v>93</v>
-      </c>
-      <c t="s" r="E35">
-        <v>29</v>
-      </c>
-    </row>
-    <row spans="1:6" r="36">
-      <c t="s" r="A36">
-        <v>143</v>
-      </c>
-      <c t="s" r="B36">
-        <v>65</v>
-      </c>
-      <c t="s" r="C36">
-        <v>50</v>
-      </c>
-      <c t="s" r="E36">
-        <v>20</v>
-      </c>
-    </row>
-    <row spans="1:6" r="37">
-      <c t="s" r="A37">
-        <v>156</v>
-      </c>
-      <c t="s" r="B37">
-        <v>77</v>
-      </c>
-      <c t="s" r="C37">
-        <v>65</v>
-      </c>
-      <c t="s" r="E37">
-        <v>3</v>
-      </c>
-    </row>
-    <row spans="1:6" r="38">
-      <c t="s" r="A38">
-        <v>146</v>
-      </c>
-      <c t="s" r="B38">
-        <v>68</v>
-      </c>
-      <c t="s" r="C38">
-        <v>77</v>
-      </c>
-      <c t="s" r="E38">
-        <v>5</v>
-      </c>
-    </row>
-    <row spans="1:6" r="39">
-      <c t="s" r="A39">
-        <v>165</v>
-      </c>
-      <c t="s" r="B39">
-        <v>84</v>
-      </c>
-      <c t="s" r="C39">
-        <v>68</v>
-      </c>
-      <c t="s" r="E39">
+      <c t="s" r="B66">
         <v>6</v>
       </c>
     </row>
-    <row spans="1:6" r="40">
-      <c t="s" r="A40">
-        <v>136</v>
-      </c>
-      <c t="s" r="B40">
-        <v>61</v>
-      </c>
-      <c t="s" r="C40">
-        <v>84</v>
-      </c>
-    </row>
-    <row spans="1:6" r="41">
-      <c t="s" r="A41">
-        <v>154</v>
-      </c>
-      <c t="s" r="B41">
-        <v>75</v>
-      </c>
-      <c t="s" r="C41">
-        <v>61</v>
-      </c>
-    </row>
-    <row spans="1:6" r="42">
-      <c t="s" r="A42">
-        <v>164</v>
-      </c>
-      <c t="s" r="B42">
-        <v>83</v>
-      </c>
-      <c t="s" r="C42">
-        <v>75</v>
-      </c>
-    </row>
-    <row spans="1:6" r="43">
-      <c t="s" r="A43">
-        <v>135</v>
-      </c>
-      <c t="s" r="B43">
-        <v>60</v>
-      </c>
-      <c t="s" r="C43">
-        <v>83</v>
-      </c>
-    </row>
-    <row spans="1:6" r="44">
-      <c t="s" r="A44">
-        <v>163</v>
-      </c>
-      <c t="s" r="B44">
-        <v>82</v>
-      </c>
-      <c t="s" r="C44">
-        <v>60</v>
-      </c>
-    </row>
-    <row spans="1:6" r="45">
-      <c t="s" r="A45">
-        <v>142</v>
-      </c>
-      <c t="s" r="B45">
-        <v>64</v>
-      </c>
-      <c t="s" r="C45">
-        <v>82</v>
-      </c>
-    </row>
-    <row spans="1:6" r="46">
-      <c t="s" r="A46">
-        <v>184</v>
-      </c>
-      <c t="s" r="B46">
-        <v>90</v>
-      </c>
-      <c t="s" r="C46">
-        <v>64</v>
-      </c>
-    </row>
-    <row spans="1:6" r="47">
-      <c t="s" r="A47">
-        <v>158</v>
-      </c>
-      <c t="s" r="B47">
-        <v>79</v>
-      </c>
-      <c t="s" r="C47">
-        <v>90</v>
-      </c>
-    </row>
-    <row spans="1:6" r="48">
-      <c t="s" r="A48">
-        <v>153</v>
-      </c>
-      <c t="s" r="B48">
-        <v>74</v>
-      </c>
-      <c t="s" r="C48">
-        <v>79</v>
-      </c>
-    </row>
-    <row spans="1:6" r="49">
-      <c t="s" r="A49">
-        <v>196</v>
-      </c>
-      <c t="s" r="B49">
-        <v>49</v>
-      </c>
-      <c t="s" r="C49">
-        <v>74</v>
-      </c>
-    </row>
-    <row spans="1:6" r="50">
-      <c t="s" r="A50">
-        <v>120</v>
-      </c>
-      <c t="s" r="B50">
-        <v>13</v>
-      </c>
-    </row>
-    <row spans="1:6" r="51">
-      <c t="s" r="A51">
-        <v>121</v>
-      </c>
-      <c t="s" r="B51">
-        <v>14</v>
-      </c>
-    </row>
-    <row spans="1:6" r="52">
-      <c t="s" r="A52">
-        <v>111</v>
-      </c>
-      <c t="s" r="B52">
-        <v>4</v>
-      </c>
-    </row>
-    <row spans="1:6" r="53">
-      <c t="s" r="A53">
-        <v>193</v>
-      </c>
-      <c t="s" r="B53">
-        <v>36</v>
-      </c>
-    </row>
-    <row spans="1:6" r="54">
-      <c t="s" r="A54">
-        <v>114</v>
-      </c>
-      <c t="s" r="B54">
-        <v>7</v>
-      </c>
-    </row>
-    <row spans="1:6" r="55">
-      <c t="s" r="A55">
-        <v>119</v>
-      </c>
-      <c t="s" r="B55">
-        <v>12</v>
-      </c>
-    </row>
-    <row spans="1:6" r="56">
-      <c t="s" r="A56">
-        <v>194</v>
-      </c>
-      <c t="s" r="B56">
-        <v>37</v>
-      </c>
-    </row>
-    <row spans="1:6" r="57">
-      <c t="s" r="A57">
-        <v>123</v>
-      </c>
-      <c t="s" r="B57">
-        <v>16</v>
-      </c>
-    </row>
-    <row spans="1:6" r="58">
-      <c t="s" r="A58">
-        <v>170</v>
-      </c>
-      <c t="s" r="B58">
-        <v>27</v>
-      </c>
-    </row>
-    <row spans="1:6" r="59">
-      <c t="s" r="A59">
-        <v>192</v>
-      </c>
-      <c t="s" r="B59">
-        <v>35</v>
-      </c>
-    </row>
-    <row spans="1:6" r="60">
-      <c t="s" r="A60">
-        <v>141</v>
-      </c>
-      <c t="s" r="B60">
-        <v>25</v>
-      </c>
-    </row>
-    <row spans="1:6" r="61">
-      <c t="s" r="A61">
-        <v>133</v>
-      </c>
-      <c t="s" r="B61">
-        <v>22</v>
-      </c>
-    </row>
-    <row spans="1:6" r="62">
-      <c t="s" r="A62">
-        <v>102</v>
-      </c>
-      <c t="s" r="B62">
-        <v>2</v>
-      </c>
-    </row>
-    <row spans="1:6" r="63">
-      <c t="s" r="A63">
-        <v>175</v>
-      </c>
-      <c t="s" r="B63">
-        <v>31</v>
-      </c>
-    </row>
-    <row spans="1:6" r="64">
-      <c t="s" r="A64">
-        <v>176</v>
-      </c>
-      <c t="s" r="B64">
-        <v>32</v>
-      </c>
-    </row>
-    <row spans="1:6" r="65">
-      <c t="s" r="A65">
-        <v>177</v>
-      </c>
-      <c t="s" r="B65">
-        <v>33</v>
-      </c>
-    </row>
-    <row spans="1:6" r="66">
-      <c t="s" r="A66">
-        <v>178</v>
-      </c>
-      <c t="s" r="B66">
-        <v>34</v>
-      </c>
-    </row>
-    <row spans="1:6" r="67">
+    <row r="67" spans="1:6">
       <c t="s" r="A67">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c t="s" r="B67">
         <v>28</v>
       </c>
     </row>
-    <row spans="1:6" r="68">
+    <row r="68" spans="1:6">
       <c t="s" r="A68">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c t="s" r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:6" r="69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c t="s" r="A69">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c t="s" r="B69">
-        <v>17</v>
-      </c>
-    </row>
-    <row spans="1:6" r="70">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c t="s" r="A70">
         <v>140</v>
       </c>
       <c t="s" r="B70">
-        <v>24</v>
-      </c>
-    </row>
-    <row spans="1:6" r="71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c t="s" r="A71">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c t="s" r="B71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c t="s" r="A72">
+        <v>151</v>
+      </c>
+      <c t="s" r="B72">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c t="s" r="A73">
+        <v>207</v>
+      </c>
+      <c t="s" r="B73">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c t="s" r="A74">
+        <v>149</v>
+      </c>
+      <c t="s" r="B74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c t="s" r="A75">
+        <v>208</v>
+      </c>
+      <c t="s" r="B75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c t="s" r="A76">
+        <v>177</v>
+      </c>
+      <c t="s" r="B76">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c t="s" r="A77">
+        <v>171</v>
+      </c>
+      <c t="s" r="B77">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c t="s" r="A78">
+        <v>138</v>
+      </c>
+      <c t="s" r="B78">
         <v>0</v>
       </c>
     </row>
-    <row spans="1:6" r="72">
-      <c t="s" r="A72">
-        <v>125</v>
-      </c>
-      <c t="s" r="B72">
+    <row r="79" spans="1:6">
+      <c t="s" r="A79">
+        <v>212</v>
+      </c>
+      <c t="s" r="B79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c t="s" r="A80">
+        <v>166</v>
+      </c>
+      <c t="s" r="B80">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c t="s" r="A81">
+        <v>210</v>
+      </c>
+      <c t="s" r="B81">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c t="s" r="A82">
+        <v>178</v>
+      </c>
+      <c t="s" r="B82">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c t="s" r="A83">
+        <v>156</v>
+      </c>
+      <c t="s" r="B83">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c t="s" r="A84">
+        <v>153</v>
+      </c>
+      <c t="s" r="B84">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c t="s" r="A85">
+        <v>161</v>
+      </c>
+      <c t="s" r="B85">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c t="s" r="A86">
+        <v>155</v>
+      </c>
+      <c t="s" r="B86">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c t="s" r="A87">
+        <v>154</v>
+      </c>
+      <c t="s" r="B87">
         <v>18</v>
       </c>
     </row>
-    <row spans="1:6" r="73">
-      <c t="s" r="A73">
-        <v>117</v>
-      </c>
-      <c t="s" r="B73">
-        <v>10</v>
-      </c>
-    </row>
-    <row spans="1:6" r="74">
-      <c t="s" r="A74">
-        <v>122</v>
-      </c>
-      <c t="s" r="B74">
-        <v>15</v>
-      </c>
-    </row>
-    <row spans="1:6" r="75">
-      <c t="s" r="A75">
-        <v>126</v>
-      </c>
-      <c t="s" r="B75">
-        <v>19</v>
-      </c>
-    </row>
-    <row spans="1:6" r="76">
-      <c t="s" r="A76">
-        <v>128</v>
-      </c>
-      <c t="s" r="B76">
-        <v>21</v>
-      </c>
-    </row>
-    <row spans="1:6" r="77">
-      <c t="s" r="A77">
-        <v>118</v>
-      </c>
-      <c t="s" r="B77">
-        <v>11</v>
-      </c>
-    </row>
-    <row spans="1:6" r="78">
-      <c t="s" r="A78">
-        <v>139</v>
-      </c>
-      <c t="s" r="B78">
-        <v>23</v>
-      </c>
-    </row>
-    <row spans="1:6" r="79">
-      <c t="s" r="A79">
-        <v>169</v>
-      </c>
-      <c t="s" r="B79">
-        <v>26</v>
-      </c>
-    </row>
-    <row spans="1:6" r="80">
-      <c t="s" r="A80">
-        <v>174</v>
-      </c>
-      <c t="s" r="B80">
-        <v>30</v>
-      </c>
-    </row>
-    <row spans="1:6" r="81">
-      <c t="s" r="A81">
-        <v>115</v>
-      </c>
-      <c t="s" r="B81">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:6" r="82">
-      <c t="s" r="A82">
-        <v>116</v>
-      </c>
-      <c t="s" r="B82">
-        <v>9</v>
-      </c>
-    </row>
-    <row spans="1:6" r="83">
-      <c t="s" r="A83">
-        <v>173</v>
-      </c>
-      <c t="s" r="B83">
-        <v>29</v>
-      </c>
-    </row>
-    <row spans="1:6" r="84">
-      <c t="s" r="A84">
-        <v>127</v>
-      </c>
-      <c t="s" r="B84">
-        <v>20</v>
-      </c>
-    </row>
-    <row spans="1:6" r="85">
-      <c t="s" r="A85">
-        <v>110</v>
-      </c>
-      <c t="s" r="B85">
-        <v>3</v>
-      </c>
-    </row>
-    <row spans="1:6" r="86">
-      <c t="s" r="A86">
-        <v>112</v>
-      </c>
-      <c t="s" r="B86">
-        <v>5</v>
-      </c>
-    </row>
-    <row spans="1:6" r="87">
-      <c t="s" r="A87">
-        <v>113</v>
-      </c>
-      <c t="s" r="B87">
-        <v>6</v>
-      </c>
-    </row>
-    <row spans="1:6" r="88">
+    <row r="88" spans="1:6">
       <c t="s" r="A88">
-        <v>103</v>
+        <v>164</v>
       </c>
       <c t="s" r="B88">
-        <v>39</v>
-      </c>
-    </row>
-    <row spans="1:6" r="89">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c t="s" r="A89">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c t="s" r="B89">
-        <v>45</v>
-      </c>
-    </row>
-    <row spans="1:6" r="90">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c t="s" r="A90">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c t="s" r="B90">
-        <v>41</v>
-      </c>
-    </row>
-    <row spans="1:6" r="91">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c t="s" r="A91">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c t="s" r="B91">
-        <v>40</v>
-      </c>
-    </row>
-    <row spans="1:6" r="92">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c t="s" r="A92">
         <v>160</v>
       </c>
       <c t="s" r="B92">
-        <v>44</v>
-      </c>
-    </row>
-    <row spans="1:6" r="93">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c t="s" r="A93">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c t="s" r="B93">
-        <v>43</v>
-      </c>
-    </row>
-    <row spans="1:6" r="94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c t="s" r="A94">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c t="s" r="B94">
-        <v>48</v>
-      </c>
-    </row>
-    <row spans="1:6" r="95">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c t="s" r="A95">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c t="s" r="B95">
-        <v>46</v>
-      </c>
-    </row>
-    <row spans="1:6" r="96">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c t="s" r="A96">
-        <v>151</v>
+        <v>230</v>
       </c>
       <c t="s" r="B96">
-        <v>42</v>
-      </c>
-    </row>
-    <row spans="1:6" r="97">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c t="s" r="A97">
-        <v>98</v>
+        <v>232</v>
       </c>
       <c t="s" r="B97">
-        <v>38</v>
-      </c>
-    </row>
-    <row spans="1:6" r="98">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c t="s" r="A98">
-        <v>168</v>
+        <v>231</v>
       </c>
       <c t="s" r="B98">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>